<commit_message>
Tap descriptions to hear audio
</commit_message>
<xml_diff>
--- a/Toddler Taxonomist/animal_list.xlsx
+++ b/Toddler Taxonomist/animal_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="0" windowWidth="28900" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="23460" yWindow="0" windowWidth="12680" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="organisms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="956">
   <si>
     <t>Common Name</t>
   </si>
@@ -2886,13 +2886,16 @@
   </si>
   <si>
     <t>The Lubber Grasshopper emits a foul-smelling and foul-tasting foamy secretion from the thorax when it is disturbed. It also lets off a loud hissing sound that can scare animals. Species of grasshoppers that change colour and behaviour at high population densities are called locusts.</t>
+  </si>
+  <si>
+    <t>Unlike other zebras, the mountain zebra has a dewlap, which is a flap of skin that hangs beneath its neck. Like all extant zebras, it is boldly striped in black and white and no two individuals look exactly alike. The stripes can be either black or dark brown and white. Their stripes cover their whole bodies except for their bellies.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2953,8 +2956,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2969,6 +2984,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3007,7 +3028,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="585">
+  <cellStyleXfs count="593">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3593,8 +3614,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3609,8 +3638,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="187" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="568"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="585">
+  <cellStyles count="593">
     <cellStyle name="Bad" xfId="568" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3904,6 +3939,10 @@
     <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4194,6 +4233,10 @@
     <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="187" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -4527,10 +4570,10 @@
   <dimension ref="A1:AC84"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Z48" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y54" sqref="Y54"/>
+      <selection pane="bottomRight" activeCell="Z52" sqref="Z52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9100,7 +9143,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="60">
+    <row r="52" spans="1:29" ht="75">
       <c r="A52" s="4" t="s">
         <v>459</v>
       </c>
@@ -9177,7 +9220,7 @@
         <v>514</v>
       </c>
       <c r="Z52" s="6" t="s">
-        <v>929</v>
+        <v>955</v>
       </c>
       <c r="AA52" s="2"/>
       <c r="AB52" t="s">
@@ -12050,8 +12093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="F11" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView showRuler="0" topLeftCell="N72" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12489,7 +12532,7 @@
       <c r="K11" t="s">
         <v>407</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="10" t="s">
         <v>40</v>
       </c>
       <c r="N11" t="s">
@@ -12589,7 +12632,7 @@
       <c r="K16" t="s">
         <v>415</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="12" t="s">
         <v>49</v>
       </c>
       <c r="N16" t="s">
@@ -12609,7 +12652,7 @@
       <c r="K17" t="s">
         <v>417</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="12" t="s">
         <v>53</v>
       </c>
       <c r="N17" t="s">
@@ -12626,7 +12669,7 @@
       <c r="K18" t="s">
         <v>447</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="M18" s="12" t="s">
         <v>53</v>
       </c>
       <c r="N18" t="s">
@@ -12643,7 +12686,7 @@
       <c r="K19" t="s">
         <v>419</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="12" t="s">
         <v>53</v>
       </c>
       <c r="N19" t="s">
@@ -12660,7 +12703,7 @@
       <c r="K20" t="s">
         <v>596</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="12" t="s">
         <v>58</v>
       </c>
       <c r="N20" t="s">
@@ -12677,7 +12720,7 @@
       <c r="K21" t="s">
         <v>423</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="12" t="s">
         <v>58</v>
       </c>
       <c r="N21" t="s">
@@ -12694,7 +12737,7 @@
       <c r="K22" t="s">
         <v>613</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="12" t="s">
         <v>58</v>
       </c>
       <c r="N22" t="s">
@@ -12815,7 +12858,7 @@
       <c r="K30" t="s">
         <v>441</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="12" t="s">
         <v>216</v>
       </c>
       <c r="N30" t="s">
@@ -12905,7 +12948,7 @@
       <c r="N36" t="s">
         <v>268</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="O36" s="13" t="s">
         <v>951</v>
       </c>
     </row>
@@ -13010,7 +13053,7 @@
       </c>
     </row>
     <row r="45" spans="11:15" ht="90">
-      <c r="M45" s="8" t="s">
+      <c r="M45" s="11" t="s">
         <v>327</v>
       </c>
       <c r="N45" t="s">
@@ -13320,7 +13363,7 @@
       </c>
     </row>
     <row r="73" spans="13:16" ht="60">
-      <c r="M73" s="8" t="s">
+      <c r="M73" s="10" t="s">
         <v>662</v>
       </c>
       <c r="N73" t="s">

</xml_diff>

<commit_message>
Fix for spelling error
</commit_message>
<xml_diff>
--- a/Toddler Taxonomist/animal_list.xlsx
+++ b/Toddler Taxonomist/animal_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="957">
   <si>
     <t>Common Name</t>
   </si>
@@ -2204,9 +2204,6 @@
     <t>http://en.wikipedia.org/wiki/Two-toed_sloth</t>
   </si>
   <si>
-    <t>Prarie Dog</t>
-  </si>
-  <si>
     <t>Black-tailed Prarie Dog</t>
   </si>
   <si>
@@ -2889,6 +2886,12 @@
   </si>
   <si>
     <t>Orca</t>
+  </si>
+  <si>
+    <t>Black-tailed Prairie Dog</t>
+  </si>
+  <si>
+    <t>Prairie Dog</t>
   </si>
 </sst>
 </file>
@@ -4570,10 +4573,10 @@
   <dimension ref="A1:AC84"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AB39" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C76" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB35" sqref="AB35"/>
+      <selection pane="bottomRight" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4690,7 +4693,7 @@
         <v>369</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="90">
@@ -4770,16 +4773,16 @@
         <v>13</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="AA2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="AB2" t="s">
         <v>368</v>
       </c>
       <c r="AC2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="60">
@@ -4859,16 +4862,16 @@
         <v>19</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AA3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="AB3" t="s">
         <v>368</v>
       </c>
       <c r="AC3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="105">
@@ -4948,16 +4951,16 @@
         <v>22</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AA4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AB4" t="s">
         <v>368</v>
       </c>
       <c r="AC4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="75">
@@ -5037,16 +5040,16 @@
         <v>23</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AA5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AB5" t="s">
         <v>370</v>
       </c>
       <c r="AC5" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="75">
@@ -5126,16 +5129,16 @@
         <v>26</v>
       </c>
       <c r="Z6" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="AA6" t="s">
         <v>748</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>749</v>
       </c>
       <c r="AB6" t="s">
         <v>370</v>
       </c>
       <c r="AC6" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="75">
@@ -5215,16 +5218,16 @@
         <v>45</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AA7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AB7" t="s">
         <v>370</v>
       </c>
       <c r="AC7" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="60">
@@ -5304,16 +5307,16 @@
         <v>29</v>
       </c>
       <c r="Z8" s="6" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AA8" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AB8" t="s">
         <v>371</v>
       </c>
       <c r="AC8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="75">
@@ -5393,16 +5396,16 @@
         <v>32</v>
       </c>
       <c r="Z9" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AA9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AB9" t="s">
         <v>371</v>
       </c>
       <c r="AC9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="75">
@@ -5482,16 +5485,16 @@
         <v>35</v>
       </c>
       <c r="Z10" s="6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="AA10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="AB10" t="s">
         <v>371</v>
       </c>
       <c r="AC10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="75">
@@ -5571,16 +5574,16 @@
         <v>38</v>
       </c>
       <c r="Z11" s="6" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AA11" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="AB11" t="s">
         <v>372</v>
       </c>
       <c r="AC11" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="45">
@@ -5657,19 +5660,19 @@
         <v>120</v>
       </c>
       <c r="Y12" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="Z12" s="6" t="s">
+        <v>876</v>
+      </c>
+      <c r="AA12" t="s">
         <v>877</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>878</v>
       </c>
       <c r="AB12" t="s">
         <v>372</v>
       </c>
       <c r="AC12" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="60">
@@ -5746,19 +5749,19 @@
         <v>121</v>
       </c>
       <c r="Y13" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="Z13" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="AA13" t="s">
         <v>879</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>880</v>
       </c>
       <c r="AB13" t="s">
         <v>372</v>
       </c>
       <c r="AC13" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="75">
@@ -5838,10 +5841,10 @@
         <v>155</v>
       </c>
       <c r="Z14" s="6" t="s">
+        <v>880</v>
+      </c>
+      <c r="AA14" t="s">
         <v>881</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>882</v>
       </c>
       <c r="AB14" t="s">
         <v>373</v>
@@ -5927,16 +5930,16 @@
         <v>50</v>
       </c>
       <c r="Z15" s="6" t="s">
+        <v>882</v>
+      </c>
+      <c r="AA15" t="s">
         <v>883</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>884</v>
       </c>
       <c r="AB15" t="s">
         <v>373</v>
       </c>
       <c r="AC15" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="75">
@@ -5944,7 +5947,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C16" t="s">
         <v>49</v>
@@ -6016,16 +6019,16 @@
         <v>52</v>
       </c>
       <c r="Z16" s="6" t="s">
+        <v>885</v>
+      </c>
+      <c r="AA16" t="s">
         <v>886</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>887</v>
       </c>
       <c r="AB16" t="s">
         <v>373</v>
       </c>
       <c r="AC16" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="75">
@@ -6105,16 +6108,16 @@
         <v>153</v>
       </c>
       <c r="Z17" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AA17" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="AB17" t="s">
         <v>374</v>
       </c>
       <c r="AC17" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="60">
@@ -6194,16 +6197,16 @@
         <v>54</v>
       </c>
       <c r="Z18" s="6" t="s">
+        <v>889</v>
+      </c>
+      <c r="AA18" t="s">
         <v>890</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>891</v>
       </c>
       <c r="AB18" t="s">
         <v>374</v>
       </c>
       <c r="AC18" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="60">
@@ -6283,16 +6286,16 @@
         <v>56</v>
       </c>
       <c r="Z19" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="AA19" t="s">
         <v>892</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>893</v>
       </c>
       <c r="AB19" t="s">
         <v>374</v>
       </c>
       <c r="AC19" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="75">
@@ -6372,16 +6375,16 @@
         <v>59</v>
       </c>
       <c r="Z20" s="6" t="s">
+        <v>893</v>
+      </c>
+      <c r="AA20" t="s">
         <v>894</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>895</v>
       </c>
       <c r="AB20" t="s">
         <v>375</v>
       </c>
       <c r="AC20" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="90">
@@ -6461,7 +6464,7 @@
         <v>157</v>
       </c>
       <c r="Z21" s="6" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="AA21" t="s">
         <v>156</v>
@@ -6470,7 +6473,7 @@
         <v>375</v>
       </c>
       <c r="AC21" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="75">
@@ -6550,16 +6553,16 @@
         <v>61</v>
       </c>
       <c r="Z22" s="6" t="s">
+        <v>895</v>
+      </c>
+      <c r="AA22" t="s">
         <v>896</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>897</v>
       </c>
       <c r="AB22" t="s">
         <v>375</v>
       </c>
       <c r="AC22" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="75">
@@ -6639,16 +6642,16 @@
         <v>87</v>
       </c>
       <c r="Z23" s="6" t="s">
+        <v>897</v>
+      </c>
+      <c r="AA23" t="s">
         <v>898</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>899</v>
       </c>
       <c r="AB23" t="s">
         <v>376</v>
       </c>
       <c r="AC23" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="75">
@@ -6728,7 +6731,7 @@
         <v>167</v>
       </c>
       <c r="Z24" s="6" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AA24" t="s">
         <v>168</v>
@@ -6737,7 +6740,7 @@
         <v>377</v>
       </c>
       <c r="AC24" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="75">
@@ -6817,7 +6820,7 @@
         <v>178</v>
       </c>
       <c r="Z25" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AA25" t="s">
         <v>179</v>
@@ -6826,7 +6829,7 @@
         <v>378</v>
       </c>
       <c r="AC25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="75">
@@ -6906,7 +6909,7 @@
         <v>189</v>
       </c>
       <c r="Z26" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AA26" t="s">
         <v>188</v>
@@ -6915,7 +6918,7 @@
         <v>378</v>
       </c>
       <c r="AC26" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="90">
@@ -6995,7 +6998,7 @@
         <v>195</v>
       </c>
       <c r="Z27" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="AA27" t="s">
         <v>192</v>
@@ -7004,7 +7007,7 @@
         <v>378</v>
       </c>
       <c r="AC27" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="75">
@@ -7084,7 +7087,7 @@
         <v>203</v>
       </c>
       <c r="Z28" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="AA28" t="s">
         <v>202</v>
@@ -7093,7 +7096,7 @@
         <v>379</v>
       </c>
       <c r="AC28" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="75">
@@ -7173,7 +7176,7 @@
         <v>213</v>
       </c>
       <c r="Z29" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AA29" t="s">
         <v>212</v>
@@ -7182,7 +7185,7 @@
         <v>377</v>
       </c>
       <c r="AC29" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="60">
@@ -7262,7 +7265,7 @@
         <v>222</v>
       </c>
       <c r="Z30" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AA30" t="s">
         <v>214</v>
@@ -7271,7 +7274,7 @@
         <v>380</v>
       </c>
       <c r="AC30" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="75">
@@ -7351,7 +7354,7 @@
         <v>226</v>
       </c>
       <c r="Z31" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="AA31" t="s">
         <v>227</v>
@@ -7360,7 +7363,7 @@
         <v>380</v>
       </c>
       <c r="AC31" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="75">
@@ -7440,7 +7443,7 @@
         <v>237</v>
       </c>
       <c r="Z32" s="6" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="AA32" t="s">
         <v>238</v>
@@ -7449,7 +7452,7 @@
         <v>381</v>
       </c>
       <c r="AC32" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="60">
@@ -7526,10 +7529,10 @@
         <v>239</v>
       </c>
       <c r="Y33" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="Z33" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="AA33" t="s">
         <v>256</v>
@@ -7538,7 +7541,7 @@
         <v>381</v>
       </c>
       <c r="AC33" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="60">
@@ -7618,7 +7621,7 @@
         <v>254</v>
       </c>
       <c r="Z34" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="AA34" t="s">
         <v>255</v>
@@ -7627,7 +7630,7 @@
         <v>527</v>
       </c>
       <c r="AC34" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="75">
@@ -7707,7 +7710,7 @@
         <v>258</v>
       </c>
       <c r="Z35" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="AA35" t="s">
         <v>259</v>
@@ -7716,7 +7719,7 @@
         <v>527</v>
       </c>
       <c r="AC35" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="60">
@@ -7796,7 +7799,7 @@
         <v>269</v>
       </c>
       <c r="Z36" s="6" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="AA36" t="s">
         <v>270</v>
@@ -7805,7 +7808,7 @@
         <v>527</v>
       </c>
       <c r="AC36" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="90">
@@ -7882,10 +7885,10 @@
         <v>276</v>
       </c>
       <c r="Y37" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="Z37" s="6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="AA37" t="s">
         <v>277</v>
@@ -7894,7 +7897,7 @@
         <v>382</v>
       </c>
       <c r="AC37" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="75">
@@ -7974,7 +7977,7 @@
         <v>281</v>
       </c>
       <c r="Z38" s="6" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="AA38" t="s">
         <v>282</v>
@@ -7983,7 +7986,7 @@
         <v>382</v>
       </c>
       <c r="AC38" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="60">
@@ -8060,10 +8063,10 @@
         <v>286</v>
       </c>
       <c r="Y39" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="Z39" s="6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="AA39" t="s">
         <v>287</v>
@@ -8072,7 +8075,7 @@
         <v>382</v>
       </c>
       <c r="AC39" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="90">
@@ -8152,7 +8155,7 @@
         <v>292</v>
       </c>
       <c r="Z40" s="6" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="AA40" t="s">
         <v>293</v>
@@ -8161,7 +8164,7 @@
         <v>382</v>
       </c>
       <c r="AC40" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="45">
@@ -8238,10 +8241,10 @@
         <v>300</v>
       </c>
       <c r="Y41" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="Z41" s="6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="AA41" t="s">
         <v>301</v>
@@ -8250,7 +8253,7 @@
         <v>377</v>
       </c>
       <c r="AC41" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="75">
@@ -8330,7 +8333,7 @@
         <v>309</v>
       </c>
       <c r="Z42" s="6" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="AA42" t="s">
         <v>310</v>
@@ -8339,7 +8342,7 @@
         <v>377</v>
       </c>
       <c r="AC42" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="75">
@@ -8419,7 +8422,7 @@
         <v>315</v>
       </c>
       <c r="Z43" s="6" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="AA43" t="s">
         <v>316</v>
@@ -8428,7 +8431,7 @@
         <v>377</v>
       </c>
       <c r="AC43" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="60">
@@ -8508,7 +8511,7 @@
         <v>324</v>
       </c>
       <c r="Z44" s="6" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="AA44" t="s">
         <v>325</v>
@@ -8517,7 +8520,7 @@
         <v>383</v>
       </c>
       <c r="AC44" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="90">
@@ -8597,7 +8600,7 @@
         <v>331</v>
       </c>
       <c r="Z45" s="6" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="AA45" t="s">
         <v>326</v>
@@ -8606,7 +8609,7 @@
         <v>383</v>
       </c>
       <c r="AC45" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="90">
@@ -8686,7 +8689,7 @@
         <v>389</v>
       </c>
       <c r="Z46" s="6" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AA46" s="2" t="s">
         <v>386</v>
@@ -8695,7 +8698,7 @@
         <v>478</v>
       </c>
       <c r="AC46" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="75">
@@ -8775,7 +8778,7 @@
         <v>390</v>
       </c>
       <c r="Z47" s="6" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AA47" s="2" t="s">
         <v>391</v>
@@ -8784,7 +8787,7 @@
         <v>377</v>
       </c>
       <c r="AC47" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="75">
@@ -8864,7 +8867,7 @@
         <v>393</v>
       </c>
       <c r="Z48" s="6" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AA48" s="2" t="s">
         <v>394</v>
@@ -8873,7 +8876,7 @@
         <v>492</v>
       </c>
       <c r="AC48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="75">
@@ -8953,7 +8956,7 @@
         <v>396</v>
       </c>
       <c r="Z49" s="6" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="AA49" s="2" t="s">
         <v>397</v>
@@ -8962,7 +8965,7 @@
         <v>504</v>
       </c>
       <c r="AC49" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="75">
@@ -9042,7 +9045,7 @@
         <v>511</v>
       </c>
       <c r="Z50" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AA50" s="2" t="s">
         <v>400</v>
@@ -9051,7 +9054,7 @@
         <v>507</v>
       </c>
       <c r="AC50" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="75">
@@ -9131,7 +9134,7 @@
         <v>517</v>
       </c>
       <c r="Z51" s="6" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="AA51" s="2" t="s">
         <v>401</v>
@@ -9140,7 +9143,7 @@
         <v>507</v>
       </c>
       <c r="AC51" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="75">
@@ -9220,14 +9223,14 @@
         <v>512</v>
       </c>
       <c r="Z52" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AA52" s="2"/>
       <c r="AB52" t="s">
         <v>507</v>
       </c>
       <c r="AC52" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="90">
@@ -9307,7 +9310,7 @@
         <v>518</v>
       </c>
       <c r="Z53" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="AA53" s="2" t="s">
         <v>403</v>
@@ -9316,7 +9319,7 @@
         <v>377</v>
       </c>
       <c r="AC53" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="60">
@@ -9396,7 +9399,7 @@
         <v>525</v>
       </c>
       <c r="Z54" s="6" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="AA54" s="2" t="s">
         <v>405</v>
@@ -9405,7 +9408,7 @@
         <v>527</v>
       </c>
       <c r="AC54" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="60">
@@ -9485,7 +9488,7 @@
         <v>534</v>
       </c>
       <c r="Z55" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AA55" s="2" t="s">
         <v>407</v>
@@ -9494,7 +9497,7 @@
         <v>527</v>
       </c>
       <c r="AC55" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="90">
@@ -9574,7 +9577,7 @@
         <v>544</v>
       </c>
       <c r="Z56" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AA56" s="2" t="s">
         <v>545</v>
@@ -9583,7 +9586,7 @@
         <v>527</v>
       </c>
       <c r="AC56" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="60">
@@ -9663,7 +9666,7 @@
         <v>556</v>
       </c>
       <c r="Z57" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AA57" s="2" t="s">
         <v>409</v>
@@ -9672,7 +9675,7 @@
         <v>527</v>
       </c>
       <c r="AC57" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="58" spans="1:29" ht="45">
@@ -9761,7 +9764,7 @@
         <v>377</v>
       </c>
       <c r="AC58" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="59" spans="1:29" ht="90">
@@ -9841,7 +9844,7 @@
         <v>571</v>
       </c>
       <c r="Z59" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AA59" s="2" t="s">
         <v>413</v>
@@ -9850,7 +9853,7 @@
         <v>377</v>
       </c>
       <c r="AC59" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="60" spans="1:29" ht="60">
@@ -9939,7 +9942,7 @@
         <v>377</v>
       </c>
       <c r="AC60" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="61" spans="1:29" ht="45">
@@ -10028,7 +10031,7 @@
         <v>492</v>
       </c>
       <c r="AC61" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="62" spans="1:29" ht="60">
@@ -10117,12 +10120,12 @@
         <v>492</v>
       </c>
       <c r="AC62" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="75">
       <c r="A63" s="4" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B63" t="s">
         <v>418</v>
@@ -10206,12 +10209,12 @@
         <v>590</v>
       </c>
       <c r="AC63" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="64" spans="1:29" ht="45">
       <c r="A64" s="4" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B64" t="s">
         <v>594</v>
@@ -10286,16 +10289,16 @@
         <v>602</v>
       </c>
       <c r="Z64" s="6" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="AA64" s="2" t="s">
         <v>421</v>
       </c>
       <c r="AB64" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AC64" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="65" spans="1:29" ht="75">
@@ -10384,7 +10387,7 @@
         <v>377</v>
       </c>
       <c r="AC65" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="66" spans="1:29" ht="45">
@@ -10473,7 +10476,7 @@
         <v>716</v>
       </c>
       <c r="AC66" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="67" spans="1:29" ht="75">
@@ -10553,7 +10556,7 @@
         <v>624</v>
       </c>
       <c r="Z67" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="AA67" s="2" t="s">
         <v>427</v>
@@ -10562,7 +10565,7 @@
         <v>627</v>
       </c>
       <c r="AC67" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="68" spans="1:29" ht="75">
@@ -10642,7 +10645,7 @@
         <v>629</v>
       </c>
       <c r="Z68" s="6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AA68" s="2" t="s">
         <v>430</v>
@@ -10651,7 +10654,7 @@
         <v>627</v>
       </c>
       <c r="AC68" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="69" spans="1:29" ht="90">
@@ -10728,10 +10731,10 @@
         <v>636</v>
       </c>
       <c r="Y69" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="Z69" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AA69" s="2" t="s">
         <v>432</v>
@@ -10740,7 +10743,7 @@
         <v>717</v>
       </c>
       <c r="AC69" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="70" spans="1:29" ht="90">
@@ -10820,7 +10823,7 @@
         <v>644</v>
       </c>
       <c r="Z70" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="AA70" s="2" t="s">
         <v>434</v>
@@ -10829,7 +10832,7 @@
         <v>718</v>
       </c>
       <c r="AC70" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="60">
@@ -10918,7 +10921,7 @@
         <v>719</v>
       </c>
       <c r="AC71" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="45">
@@ -11007,7 +11010,7 @@
         <v>720</v>
       </c>
       <c r="AC72" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="60">
@@ -11096,7 +11099,7 @@
         <v>721</v>
       </c>
       <c r="AC73" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="74" spans="1:29" ht="60">
@@ -11173,7 +11176,7 @@
         <v>672</v>
       </c>
       <c r="Y74" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="Z74" s="6" t="s">
         <v>673</v>
@@ -11185,7 +11188,7 @@
         <v>721</v>
       </c>
       <c r="AC74" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="75" spans="1:29" ht="60">
@@ -11271,10 +11274,10 @@
         <v>678</v>
       </c>
       <c r="AB75" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="AC75" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="90">
@@ -11354,7 +11357,7 @@
         <v>683</v>
       </c>
       <c r="Z76" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="AA76" s="2" t="s">
         <v>443</v>
@@ -11363,7 +11366,7 @@
         <v>722</v>
       </c>
       <c r="AC76" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="77" spans="1:29" ht="60">
@@ -11440,7 +11443,7 @@
         <v>688</v>
       </c>
       <c r="Y77" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="Z77" s="6" t="s">
         <v>689</v>
@@ -11452,7 +11455,7 @@
         <v>723</v>
       </c>
       <c r="AC77" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="78" spans="1:29" ht="45">
@@ -11541,7 +11544,7 @@
         <v>527</v>
       </c>
       <c r="AC78" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="79" spans="1:29" ht="45">
@@ -11618,7 +11621,7 @@
         <v>705</v>
       </c>
       <c r="Y79" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="Z79" s="6" t="s">
         <v>706</v>
@@ -11630,7 +11633,7 @@
         <v>724</v>
       </c>
       <c r="AC79" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="80" spans="1:29" ht="75">
@@ -11707,7 +11710,7 @@
         <v>711</v>
       </c>
       <c r="Y80" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="Z80" s="6" t="s">
         <v>712</v>
@@ -11719,7 +11722,7 @@
         <v>725</v>
       </c>
       <c r="AC80" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="81" spans="1:29" ht="60">
@@ -11808,18 +11811,18 @@
         <v>485</v>
       </c>
       <c r="AC81" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="82" spans="1:29" ht="75">
       <c r="A82" s="4" t="s">
-        <v>727</v>
+        <v>956</v>
       </c>
       <c r="B82" t="s">
+        <v>955</v>
+      </c>
+      <c r="C82" t="s">
         <v>728</v>
-      </c>
-      <c r="C82" t="s">
-        <v>729</v>
       </c>
       <c r="D82" t="s">
         <v>72</v>
@@ -11846,16 +11849,16 @@
         <v>106</v>
       </c>
       <c r="L82" t="s">
+        <v>729</v>
+      </c>
+      <c r="M82" t="s">
+        <v>106</v>
+      </c>
+      <c r="N82" t="s">
         <v>730</v>
       </c>
-      <c r="M82" t="s">
-        <v>106</v>
-      </c>
-      <c r="N82" t="s">
+      <c r="O82" t="s">
         <v>731</v>
-      </c>
-      <c r="O82" t="s">
-        <v>732</v>
       </c>
       <c r="P82" t="s">
         <v>106</v>
@@ -11882,33 +11885,33 @@
         <v>15</v>
       </c>
       <c r="X82" t="s">
+        <v>732</v>
+      </c>
+      <c r="Y82" t="s">
         <v>733</v>
       </c>
-      <c r="Y82" t="s">
+      <c r="Z82" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="AA82" t="s">
         <v>734</v>
       </c>
-      <c r="Z82" s="6" t="s">
-        <v>737</v>
-      </c>
-      <c r="AA82" t="s">
+      <c r="AB82" t="s">
         <v>735</v>
       </c>
-      <c r="AB82" t="s">
-        <v>736</v>
-      </c>
       <c r="AC82" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="83" spans="1:29" ht="75">
       <c r="A83" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="B83" t="s">
         <v>759</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>760</v>
-      </c>
-      <c r="C83" t="s">
-        <v>761</v>
       </c>
       <c r="D83" t="s">
         <v>72</v>
@@ -11929,22 +11932,22 @@
         <v>106</v>
       </c>
       <c r="J83" t="s">
+        <v>761</v>
+      </c>
+      <c r="K83" t="s">
+        <v>106</v>
+      </c>
+      <c r="L83" t="s">
         <v>762</v>
       </c>
-      <c r="K83" t="s">
-        <v>106</v>
-      </c>
-      <c r="L83" t="s">
+      <c r="M83" t="s">
         <v>763</v>
       </c>
-      <c r="M83" t="s">
+      <c r="N83" t="s">
         <v>764</v>
       </c>
-      <c r="N83" t="s">
+      <c r="O83" t="s">
         <v>765</v>
-      </c>
-      <c r="O83" t="s">
-        <v>766</v>
       </c>
       <c r="P83" t="s">
         <v>106</v>
@@ -11971,33 +11974,33 @@
         <v>14</v>
       </c>
       <c r="X83" t="s">
+        <v>766</v>
+      </c>
+      <c r="Y83" t="s">
         <v>767</v>
       </c>
-      <c r="Y83" t="s">
+      <c r="Z83" s="6" t="s">
         <v>768</v>
       </c>
-      <c r="Z83" s="6" t="s">
-        <v>769</v>
-      </c>
       <c r="AA83" t="s">
+        <v>783</v>
+      </c>
+      <c r="AB83" t="s">
         <v>784</v>
       </c>
-      <c r="AB83" t="s">
-        <v>785</v>
-      </c>
       <c r="AC83" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="75">
       <c r="A84" s="7" t="s">
+        <v>769</v>
+      </c>
+      <c r="B84" t="s">
         <v>770</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>771</v>
-      </c>
-      <c r="C84" t="s">
-        <v>772</v>
       </c>
       <c r="D84" t="s">
         <v>72</v>
@@ -12006,34 +12009,34 @@
         <v>246</v>
       </c>
       <c r="F84" t="s">
+        <v>772</v>
+      </c>
+      <c r="G84" t="s">
+        <v>106</v>
+      </c>
+      <c r="H84" t="s">
+        <v>106</v>
+      </c>
+      <c r="I84" t="s">
+        <v>106</v>
+      </c>
+      <c r="J84" t="s">
         <v>773</v>
       </c>
-      <c r="G84" t="s">
-        <v>106</v>
-      </c>
-      <c r="H84" t="s">
-        <v>106</v>
-      </c>
-      <c r="I84" t="s">
-        <v>106</v>
-      </c>
-      <c r="J84" t="s">
+      <c r="K84" t="s">
         <v>774</v>
       </c>
-      <c r="K84" t="s">
+      <c r="L84" t="s">
         <v>775</v>
       </c>
-      <c r="L84" t="s">
+      <c r="M84" t="s">
+        <v>106</v>
+      </c>
+      <c r="N84" t="s">
         <v>776</v>
       </c>
-      <c r="M84" t="s">
-        <v>106</v>
-      </c>
-      <c r="N84" t="s">
+      <c r="O84" t="s">
         <v>777</v>
-      </c>
-      <c r="O84" t="s">
-        <v>778</v>
       </c>
       <c r="P84" t="s">
         <v>106</v>
@@ -12060,22 +12063,22 @@
         <v>15</v>
       </c>
       <c r="X84" t="s">
+        <v>778</v>
+      </c>
+      <c r="Y84" t="s">
         <v>779</v>
       </c>
-      <c r="Y84" t="s">
+      <c r="Z84" s="6" t="s">
         <v>780</v>
       </c>
-      <c r="Z84" s="6" t="s">
+      <c r="AA84" t="s">
         <v>781</v>
       </c>
-      <c r="AA84" t="s">
+      <c r="AB84" t="s">
         <v>782</v>
       </c>
-      <c r="AB84" t="s">
-        <v>783</v>
-      </c>
       <c r="AC84" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -12121,13 +12124,13 @@
         <v>344</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>944</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>945</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>946</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>94</v>
@@ -12176,7 +12179,7 @@
         <v>110</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="60">
@@ -12204,7 +12207,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="K3" t="s">
         <v>452</v>
@@ -12216,7 +12219,7 @@
         <v>111</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="105">
@@ -12256,7 +12259,7 @@
         <v>112</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="75">
@@ -12296,7 +12299,7 @@
         <v>113</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="75">
@@ -12330,7 +12333,7 @@
         <v>399</v>
       </c>
       <c r="L6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>27</v>
@@ -12339,7 +12342,7 @@
         <v>114</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="75">
@@ -12379,7 +12382,7 @@
         <v>115</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="60">
@@ -12419,7 +12422,7 @@
         <v>116</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="75">
@@ -12447,7 +12450,7 @@
         <v>83</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="K9" t="s">
         <v>402</v>
@@ -12459,7 +12462,7 @@
         <v>117</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="75">
@@ -12487,7 +12490,7 @@
         <v>158</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="K10" t="s">
         <v>528</v>
@@ -12499,7 +12502,7 @@
         <v>118</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="75">
@@ -12539,7 +12542,7 @@
         <v>119</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="45">
@@ -12559,7 +12562,7 @@
         <v>120</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="60">
@@ -12579,7 +12582,7 @@
         <v>121</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="75">
@@ -12599,7 +12602,7 @@
         <v>122</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="60">
@@ -12619,7 +12622,7 @@
         <v>123</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="75">
@@ -12627,7 +12630,7 @@
         <v>271</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="K16" t="s">
         <v>414</v>
@@ -12639,7 +12642,7 @@
         <v>124</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="17" spans="9:15" ht="75">
@@ -12659,12 +12662,12 @@
         <v>125</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="18" spans="9:15" ht="60">
       <c r="J18" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="K18" t="s">
         <v>446</v>
@@ -12676,7 +12679,7 @@
         <v>126</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="19" spans="9:15" ht="60">
@@ -12693,7 +12696,7 @@
         <v>127</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="20" spans="9:15" ht="75">
@@ -12710,7 +12713,7 @@
         <v>128</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="21" spans="9:15" ht="90">
@@ -12727,7 +12730,7 @@
         <v>129</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="22" spans="9:15" ht="75">
@@ -12744,7 +12747,7 @@
         <v>130</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="23" spans="9:15" ht="75">
@@ -12761,7 +12764,7 @@
         <v>131</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="24" spans="9:15" ht="75">
@@ -12778,7 +12781,7 @@
         <v>166</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="25" spans="9:15" ht="75">
@@ -12795,7 +12798,7 @@
         <v>177</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="26" spans="9:15" ht="75">
@@ -12809,7 +12812,7 @@
         <v>187</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="27" spans="9:15" ht="90">
@@ -12823,7 +12826,7 @@
         <v>191</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="28" spans="9:15" ht="75">
@@ -12837,7 +12840,7 @@
         <v>201</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="29" spans="9:15" ht="75">
@@ -12851,7 +12854,7 @@
         <v>211</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="30" spans="9:15" ht="60">
@@ -12865,7 +12868,7 @@
         <v>221</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="31" spans="9:15" ht="75">
@@ -12879,7 +12882,7 @@
         <v>225</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="32" spans="9:15" ht="75">
@@ -12893,7 +12896,7 @@
         <v>236</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="33" spans="11:15" ht="60">
@@ -12907,7 +12910,7 @@
         <v>239</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="34" spans="11:15" ht="60">
@@ -12921,7 +12924,7 @@
         <v>253</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="35" spans="11:15" ht="75">
@@ -12935,7 +12938,7 @@
         <v>260</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="36" spans="11:15" ht="60">
@@ -12949,7 +12952,7 @@
         <v>268</v>
       </c>
       <c r="O36" s="13" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="37" spans="11:15" ht="90">
@@ -12963,12 +12966,12 @@
         <v>276</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="38" spans="11:15" ht="75">
       <c r="K38" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>278</v>
@@ -12977,12 +12980,12 @@
         <v>280</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="39" spans="11:15" ht="60">
       <c r="K39" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>283</v>
@@ -12991,12 +12994,12 @@
         <v>286</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="40" spans="11:15" ht="90">
       <c r="K40" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="M40" s="8" t="s">
         <v>288</v>
@@ -13005,7 +13008,7 @@
         <v>291</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="41" spans="11:15" ht="45">
@@ -13016,7 +13019,7 @@
         <v>300</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="42" spans="11:15" ht="75">
@@ -13027,7 +13030,7 @@
         <v>308</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="43" spans="11:15" ht="75">
@@ -13038,7 +13041,7 @@
         <v>314</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="44" spans="11:15" ht="60">
@@ -13049,7 +13052,7 @@
         <v>323</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="45" spans="11:15" ht="90">
@@ -13060,7 +13063,7 @@
         <v>330</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="46" spans="11:15" ht="90">
@@ -13071,7 +13074,7 @@
         <v>471</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="47" spans="11:15" ht="75">
@@ -13082,7 +13085,7 @@
         <v>477</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="48" spans="11:15" ht="75">
@@ -13093,7 +13096,7 @@
         <v>491</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="49" spans="13:16" ht="75">
@@ -13104,7 +13107,7 @@
         <v>503</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="50" spans="13:16" ht="75">
@@ -13115,7 +13118,7 @@
         <v>510</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="51" spans="13:16" ht="75">
@@ -13126,7 +13129,7 @@
         <v>516</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="52" spans="13:16" ht="60">
@@ -13137,7 +13140,7 @@
         <v>508</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="53" spans="13:16" ht="90">
@@ -13148,7 +13151,7 @@
         <v>519</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="54" spans="13:16" ht="60">
@@ -13159,7 +13162,7 @@
         <v>526</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="P54" s="9"/>
     </row>
@@ -13171,7 +13174,7 @@
         <v>535</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="56" spans="13:16" ht="90">
@@ -13182,7 +13185,7 @@
         <v>543</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="57" spans="13:16" ht="60">
@@ -13193,7 +13196,7 @@
         <v>555</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="58" spans="13:16" ht="45">
@@ -13215,7 +13218,7 @@
         <v>570</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="60" spans="13:16" ht="60">
@@ -13304,7 +13307,7 @@
         <v>623</v>
       </c>
       <c r="O67" s="6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="68" spans="13:16" ht="75">
@@ -13315,7 +13318,7 @@
         <v>628</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="69" spans="13:16" ht="90">
@@ -13326,7 +13329,7 @@
         <v>636</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="70" spans="13:16" ht="90">
@@ -13337,7 +13340,7 @@
         <v>643</v>
       </c>
       <c r="O70" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="71" spans="13:16" ht="60">
@@ -13403,7 +13406,7 @@
         <v>682</v>
       </c>
       <c r="O76" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="77" spans="13:16" ht="60">
@@ -13462,40 +13465,40 @@
         <v>713</v>
       </c>
       <c r="P81" s="9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="82" spans="13:16" ht="75">
       <c r="M82" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="N82" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="O82" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="83" spans="13:16" ht="75">
       <c r="M83" s="8" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N83" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="O83" s="6" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="84" spans="13:16" ht="75">
       <c r="M84" s="8" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="N84" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="O84" s="6" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>